<commit_message>
Avaliações AV Wyden UniRuy 2025.2 - 01122025 ...
</commit_message>
<xml_diff>
--- a/03 Assessments/Turma Java POO - 3006 Wyden UniRuy 2025_2.xlsx
+++ b/03 Assessments/Turma Java POO - 3006 Wyden UniRuy 2025_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heleno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADADA4D-297B-4381-9C64-1B0F1EC6582E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CD852B-D9F0-466B-85E3-6DB25714998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{DD6ED3E7-57DF-4A52-9E4C-63B0F7661B3D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>202402533584 - BRENO DE JESUS GUIMARAES</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>https://agendacompromisso-production.up.railway.app/; https://github.com/tamarsp/AgendaCompromisso</t>
+  </si>
+  <si>
+    <t>https://github.com/IgorSantos26/Estoque-sobrevivencia</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -524,6 +527,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0212B8F-44EC-4B38-84EB-21D2846DA7CB}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="84.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1033,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
@@ -1049,14 +1053,14 @@
         <v>0.4</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="1"/>
-        <v>2.5454545454545454</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>28</v>
+        <v>5.545454545454545</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -1246,7 +1250,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
@@ -1266,14 +1270,14 @@
         <v>0.4</v>
       </c>
       <c r="G13" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="1"/>
-        <v>8.545454545454545</v>
+        <v>5.545454545454545</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>